<commit_message>
periodic commit, has the for loop filtering individual bridge elements out of the larger concatenated dataframe known as df_data- and putting them into a dictionary of dataframes woirking.
</commit_message>
<xml_diff>
--- a/Col_El.xlsx
+++ b/Col_El.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\CodingBootcamp\Homework\CAL_BridgeData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3423996C-A139-44B2-B3B7-103F9D4DC81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D62AAB0-AA24-4901-99E3-6FEF74D72D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C70E026D-9C60-4AD4-BE8E-5E8F6FC8DAC0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C70E026D-9C60-4AD4-BE8E-5E8F6FC8DAC0}"/>
   </bookViews>
   <sheets>
     <sheet name="El_cols" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="250">
   <si>
     <t>Column1</t>
   </si>
@@ -804,7 +804,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -812,16 +812,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -829,18 +841,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -862,21 +892,23 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{AE52A113-0D4A-4D78-BBD9-2B02A15640B6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="3">
-    <queryTableFields count="2">
+  <queryTableRefresh nextId="4" unboundColumnsRight="1">
+    <queryTableFields count="3">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
       <queryTableField id="2" name="Column2" tableColumnId="2"/>
+      <queryTableField id="3" dataBound="0" tableColumnId="3"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8264C92C-AB5B-493C-9C09-8DE12BC26B61}" name="El_cols" displayName="El_cols" ref="A1:B125" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B125" xr:uid="{8264C92C-AB5B-493C-9C09-8DE12BC26B61}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{47BD2401-2010-4CAE-9FA9-94119C9E9456}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{056127D7-8AEB-4147-84D8-97015C516C02}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8264C92C-AB5B-493C-9C09-8DE12BC26B61}" name="El_cols" displayName="El_cols" ref="A1:C125" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C125" xr:uid="{8264C92C-AB5B-493C-9C09-8DE12BC26B61}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{47BD2401-2010-4CAE-9FA9-94119C9E9456}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{056127D7-8AEB-4147-84D8-97015C516C02}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{AADCF2BB-12DB-4F18-83A1-F26CE930CA4E}" uniqueName="3" name=" 'deck_rc'," queryTableFieldId="3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1179,9 +1211,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3AE1F9A-75CC-46B0-B13C-5B2E66031252}">
-  <dimension ref="A1:B125"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="C124" sqref="C1:D124"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1189,1007 +1223,1753 @@
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="C13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="1" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="C14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="1" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="C15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="1" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="C16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="1" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="C17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="C18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="1" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="C19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="1" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="C20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="1" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="C21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="1" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="C22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="1" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="C23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="1" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="C24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="1" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="C25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="1" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="C26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="1" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="C27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="1" t="s">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="C28" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="1" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="C29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="1" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+      <c r="C30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="1" t="s">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="C31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="1" t="s">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+      <c r="C32" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="1" t="s">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="C33" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="1" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="C34" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="1" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="C35" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="1" t="s">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="C36" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="1" t="s">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+      <c r="C37" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="1" t="s">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="C38" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="1" t="s">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+      <c r="C39" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="1" t="s">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+      <c r="C40" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="1" t="s">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+      <c r="C41" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="1" t="s">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+      <c r="C42" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="1" t="s">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+      <c r="C43" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="1" t="s">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+      <c r="C44" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="1" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+      <c r="C45" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="1" t="s">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="C46" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="1" t="s">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+      <c r="C47" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="1" t="s">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+      <c r="C48" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B49" s="1" t="s">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+      <c r="C49" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B50" s="1" t="s">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+      <c r="C50" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="1" t="s">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+      <c r="C51" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="1" t="s">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+      <c r="C52" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="1" t="s">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+      <c r="C53" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B54" s="1" t="s">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+      <c r="C54" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="1" t="s">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+      <c r="C55" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="1" t="s">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+      <c r="C56" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B57" s="1" t="s">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+      <c r="C57" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B58" s="1" t="s">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+      <c r="C58" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B59" s="1" t="s">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+      <c r="C59" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B60" s="1" t="s">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+      <c r="C60" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B61" s="1" t="s">
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+      <c r="C61" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B62" s="1" t="s">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+      <c r="C62" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B63" s="1" t="s">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+      <c r="C63" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B64" s="1" t="s">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+      <c r="C64" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B65" s="1" t="s">
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+      <c r="C65" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B66" s="1" t="s">
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+      <c r="C66" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B67" s="1" t="s">
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+      <c r="C67" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B68" s="1" t="s">
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
+      <c r="C68" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B69" s="1" t="s">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+      <c r="C69" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B70" s="1" t="s">
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+      <c r="C70" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B71" s="1" t="s">
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+      <c r="C71" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B72" s="1" t="s">
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+      <c r="C72" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B73" s="1" t="s">
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>144</v>
+      </c>
+      <c r="B73" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+      <c r="C73" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B74" s="1" t="s">
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
+      <c r="C74" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B75" s="1" t="s">
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+      <c r="C75" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B76" s="1" t="s">
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+      <c r="C76" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D76" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B77" s="1" t="s">
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+      <c r="C77" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B78" s="1" t="s">
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
+      <c r="C78" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B79" s="1" t="s">
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
+      <c r="C79" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B80" s="1" t="s">
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
+      <c r="C80" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B81" s="1" t="s">
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
+      <c r="C81" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B82" s="1" t="s">
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
+      <c r="C82" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D82" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B83" s="1" t="s">
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
+      <c r="C83" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B84" s="1" t="s">
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+      <c r="C84" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B85" s="1" t="s">
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
+      <c r="C85" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B86" s="1" t="s">
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
+      <c r="C86" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B87" s="1" t="s">
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
+      <c r="C87" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B88" s="1" t="s">
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
+      <c r="C88" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D88" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B89" s="1" t="s">
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
+      <c r="C89" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B90" s="1" t="s">
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
+      <c r="C90" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D90" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B91" s="1" t="s">
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
+      <c r="C91" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B92" s="1" t="s">
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
+      <c r="C92" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D92" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B93" s="1" t="s">
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" s="1" t="s">
+      <c r="C93" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B94" s="1" t="s">
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>186</v>
+      </c>
+      <c r="B94" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" s="1" t="s">
+      <c r="C94" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D94" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B95" s="1" t="s">
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
+      <c r="C95" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D95" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B96" s="1" t="s">
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>190</v>
+      </c>
+      <c r="B96" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
+      <c r="C96" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D96" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B97" s="1" t="s">
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
+      <c r="C97" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B98" s="1" t="s">
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>194</v>
+      </c>
+      <c r="B98" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
+      <c r="C98" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D98" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B99" s="1" t="s">
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>196</v>
+      </c>
+      <c r="B99" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="1" t="s">
+      <c r="C99" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B100" s="1" t="s">
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="1" t="s">
+      <c r="C100" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D100" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B101" s="1" t="s">
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" s="1" t="s">
+      <c r="C101" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B102" s="1" t="s">
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>202</v>
+      </c>
+      <c r="B102" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" s="1" t="s">
+      <c r="C102" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D102" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B103" s="1" t="s">
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>204</v>
+      </c>
+      <c r="B103" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" s="1" t="s">
+      <c r="C103" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B104" s="1" t="s">
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>206</v>
+      </c>
+      <c r="B104" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" s="1" t="s">
+      <c r="C104" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D104" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B105" s="1" t="s">
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>208</v>
+      </c>
+      <c r="B105" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="1" t="s">
+      <c r="C105" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B106" s="1" t="s">
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>210</v>
+      </c>
+      <c r="B106" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="1" t="s">
+      <c r="C106" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D106" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B107" s="1" t="s">
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>212</v>
+      </c>
+      <c r="B107" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="1" t="s">
+      <c r="C107" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D107" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B108" s="1" t="s">
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>214</v>
+      </c>
+      <c r="B108" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="1" t="s">
+      <c r="C108" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D108" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B109" s="1" t="s">
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>216</v>
+      </c>
+      <c r="B109" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" s="1" t="s">
+      <c r="C109" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B110" s="1" t="s">
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>218</v>
+      </c>
+      <c r="B110" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
+      <c r="C110" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D110" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B111" s="1" t="s">
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>220</v>
+      </c>
+      <c r="B111" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
+      <c r="C111" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="D111" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B112" s="1" t="s">
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>222</v>
+      </c>
+      <c r="B112" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" s="1" t="s">
+      <c r="C112" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D112" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B113" s="1" t="s">
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>224</v>
+      </c>
+      <c r="B113" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114" s="1" t="s">
+      <c r="C113" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B114" s="1" t="s">
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>226</v>
+      </c>
+      <c r="B114" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" s="1" t="s">
+      <c r="C114" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D114" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B115" s="1" t="s">
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>228</v>
+      </c>
+      <c r="B115" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
+      <c r="C115" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B116" s="1" t="s">
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>230</v>
+      </c>
+      <c r="B116" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
+      <c r="C116" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D116" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B117" s="1" t="s">
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>232</v>
+      </c>
+      <c r="B117" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="1" t="s">
+      <c r="C117" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B118" s="1" t="s">
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>234</v>
+      </c>
+      <c r="B118" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
+      <c r="C118" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D118" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B119" s="1" t="s">
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>236</v>
+      </c>
+      <c r="B119" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="1" t="s">
+      <c r="C119" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B120" s="1" t="s">
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>238</v>
+      </c>
+      <c r="B120" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="1" t="s">
+      <c r="C120" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D120" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B121" s="1" t="s">
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>240</v>
+      </c>
+      <c r="B121" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="1" t="s">
+      <c r="C121" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D121" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B122" s="1" t="s">
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>242</v>
+      </c>
+      <c r="B122" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" s="1" t="s">
+      <c r="C122" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D122" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B123" s="1" t="s">
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>244</v>
+      </c>
+      <c r="B123" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="1" t="s">
+      <c r="C123" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B124" s="1" t="s">
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>246</v>
+      </c>
+      <c r="B124" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" s="1" t="s">
+      <c r="C124" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D124" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="B125" s="1" t="s">
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>248</v>
+      </c>
+      <c r="B125" t="s">
         <v>249</v>
       </c>
+      <c r="C125" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>